<commit_message>
clone de la ligne option produit
</commit_message>
<xml_diff>
--- a/Soutenance/Plan de tests.xlsx
+++ b/Soutenance/Plan de tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Script_fetch" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
   <si>
     <t xml:space="preserve">Fichier JS</t>
   </si>
@@ -53,10 +53,10 @@
     <t xml:space="preserve">La fonction doit retourner 1 si le mot passé en paramètre est un mot (pas de chiffre, caractères accentués, symboles ...), et retourner 0 si ce n'en est pas un</t>
   </si>
   <si>
-    <t xml:space="preserve">Appeller la fonction avec différentes valeurs de tests (valeurs limites, valeur vide...), et on observe la valeur retournée, avec un console.log par exemple</t>
+    <t xml:space="preserve">Appeler la fonction avec différentes valeurs de tests (valeurs limites, valeur vide...), et on observe la valeur retournée, avec un console.log par exemple</t>
   </si>
   <si>
-    <t xml:space="preserve">La valeur retournée pourrait être érronée (0 au lieu de 1;  et 1 au lieu de 0)</t>
+    <t xml:space="preserve">La valeur retournée pourrait être erronée (0 au lieu de 1;  et 1 au lieu de 0)</t>
   </si>
   <si>
     <t xml:space="preserve">exemple</t>
@@ -80,16 +80,31 @@
     <t xml:space="preserve">s’il n’y a pas de data, un message est affiché dans la console.</t>
   </si>
   <si>
-    <t xml:space="preserve">15 à 23</t>
+    <t xml:space="preserve">16 à 26</t>
   </si>
   <si>
     <t xml:space="preserve">fetchProduct </t>
   </si>
   <si>
-    <t xml:space="preserve">la fonction récupére l’ensembel des valeurs contenues dans la page produit correspondant à apiLink. Il envoie également vers la page produit l’identifiant du produit sélectionné</t>
+    <t xml:space="preserve">la fonction récupère l’ensemble des valeurs contenues dans la page produit correspondant à apiLink. Il envoie également vers la page produit l’identifiant du produit sélectionné. C’est ce produit qui doit ensuite s’afficher dans la page produit</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">29 à 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fetchAffichagePanier </t>
+  </si>
+  <si>
+    <t xml:space="preserve">la fonction récupère l’ensemble des valeurs contenues dans l’api puis les envoie dans la fonction panier explorer qui croise avec les id avec le localstorage pour afficher les produits sélectionnés dans le panier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vérifier si les données affichées correspondent à celles du serveur et du localstorage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appeller la fonction avec différentes valeurs de tests (valeurs limites, valeur vide...), et on observe la valeur retournée, avec un console.log par exemple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La valeur retournée pourrait être érronée (0 au lieu de 1;  et 1 au lieu de 0)</t>
   </si>
   <si>
     <t xml:space="preserve">script_generique.js</t>
@@ -498,10 +513,10 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -582,7 +597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="37.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
@@ -602,7 +617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
@@ -624,10 +639,20 @@
     </row>
     <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="F6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5613,10 +5638,10 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5688,10 +5713,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>12</v>
@@ -5699,251 +5724,275 @@
     </row>
     <row r="4" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B4" s="8" t="n">
         <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B5" s="8" t="n">
         <v>19</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B6" s="8" t="n">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="49.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B7" s="8" t="n">
         <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B9" s="8" t="n">
         <v>23</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B10" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="B11" s="8" t="n">
         <v>25</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" customFormat="false" ht="78.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="77.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="B12" s="8" t="n">
         <v>26</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="53" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="51.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="B13" s="8" t="n">
         <v>27</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="B14" s="8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="B15" s="8" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="B16" s="8" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="B17" s="8" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="B18" s="8" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F18" s="3"/>
     </row>

</xml_diff>

<commit_message>
mise à jour total option
</commit_message>
<xml_diff>
--- a/Soutenance/Plan de tests.xlsx
+++ b/Soutenance/Plan de tests.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="97">
   <si>
     <t xml:space="preserve">Fichier JS</t>
   </si>
@@ -94,16 +94,28 @@
     <t xml:space="preserve">théorique pas d’erreur sauf si un produit du panier n’a pas d’id dans l’api (modification des données de l’api entre temps?)</t>
   </si>
   <si>
-    <t xml:space="preserve">33 à 63</t>
+    <t xml:space="preserve">33 à 72</t>
   </si>
   <si>
     <t xml:space="preserve">panierProductOption(param_produit, param_where)</t>
   </si>
   <si>
-    <t xml:space="preserve">la fonction affiche les options des différents produits dans la vignette liée au produit</t>
+    <t xml:space="preserve">la fonction affiche les options des différents produits dans la vignette liée au produit. Les attribut keyId doit contenir l’id du produit et keyOption doivent contenir le rang de l’’option dans la fiche produit de l’api</t>
   </si>
   <si>
     <t xml:space="preserve">ajouter des produits au panier et vérifier si cela s’affiche correctement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75 à 94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">panierRemoveOption=(param_cible,param_id,param_option) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">la fonction supprime une ligne d’option du panier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saisir des id et des options directement et vérifier si les couples existants son param_id / param_option  sont supprimés. param_cible correspond à l’input qui tombe à 0. il a les même param_id et param_option que le labet et la div à supprimer</t>
   </si>
   <si>
     <t xml:space="preserve">Appeler la fonction avec différentes valeurs de tests (valeurs limites, valeur vide...), et on observe la valeur retournée, avec un console.log par exemple</t>
@@ -560,7 +572,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -691,10 +703,19 @@
       </c>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
+    <row r="7" customFormat="false" ht="89.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="F7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5766,10 +5787,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>12</v>
@@ -5777,59 +5798,59 @@
     </row>
     <row r="4" customFormat="false" ht="37.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="B5" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="B6" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F6" s="15"/>
     </row>
@@ -10902,275 +10923,275 @@
     </row>
     <row r="4" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>18</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>19</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>20</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="49.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>22</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>23</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>24</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>25</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="77.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>26</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="51.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>27</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F18" s="7"/>
     </row>

</xml_diff>

<commit_message>
mise à jour script
</commit_message>
<xml_diff>
--- a/Soutenance/Plan de tests.xlsx
+++ b/Soutenance/Plan de tests.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="104">
   <si>
     <t xml:space="preserve">Fichier JS</t>
   </si>
@@ -64,10 +64,40 @@
     <t xml:space="preserve">exemple</t>
   </si>
   <si>
+    <t xml:space="preserve">page index</t>
+  </si>
+  <si>
     <t xml:space="preserve">script_template.js</t>
   </si>
   <si>
-    <t xml:space="preserve">2à16</t>
+    <t xml:space="preserve">2 à15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">index(param_fetchdata) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">la fonction affiche tous les produits contenus dans l’api. S’il y a déjà des produits ajoutés dans le panier, il affiche le nombre de modèle dans le bouton accéder au panier (appel de la fonction : compteProduitsDuPanier)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en comparant les produits affiché avec les données de l’Api</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s’il y a un problème, rien n’est affiché sur la page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17à46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productData(param_copy, param_produit, param_body) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cette fonction est appelée par index. Elle crée les cartes pour les produits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comparer ce qui est affiché dans une carte avec ce qu’il y a pour le même produit dans l’api</t>
+  </si>
+  <si>
+    <t xml:space="preserve">page panier</t>
   </si>
   <si>
     <t xml:space="preserve">supprimerUnProduitDuPanier </t>
@@ -77,9 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve">ajouter des produits au panier et clicker sur leur bouton pour voir si c’est supprimé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 à 30</t>
   </si>
   <si>
     <t xml:space="preserve">videPanier ((param_fetchdata)</t>
@@ -94,9 +121,6 @@
     <t xml:space="preserve">théorique pas d’erreur sauf si un produit du panier n’a pas d’id dans l’api (modification des données de l’api entre temps?)</t>
   </si>
   <si>
-    <t xml:space="preserve">33 à 72</t>
-  </si>
-  <si>
     <t xml:space="preserve">panierProductOption(param_produit, param_where)</t>
   </si>
   <si>
@@ -104,9 +128,6 @@
   </si>
   <si>
     <t xml:space="preserve">ajouter des produits au panier et vérifier si cela s’affiche correctement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75 à 94</t>
   </si>
   <si>
     <t xml:space="preserve">panierRemoveOption=(param_cible,param_id,param_option) </t>
@@ -367,7 +388,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,6 +405,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -421,29 +448,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -455,19 +482,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -484,6 +511,26 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -543,7 +590,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -567,63 +614,64 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1008"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="92.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="50.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="36.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="92.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="50.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="36.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="14.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="6"/>
@@ -646,195 +694,191 @@
       <c r="E3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" s="11" customFormat="true" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" customFormat="false" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="F8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="13" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="12" t="s">
+    </row>
+    <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" s="11" customFormat="true" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="13" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" customFormat="false" ht="89.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="E12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="16"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C9" s="16"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="16"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C11" s="16"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="16"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="12"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
+      <c r="F13" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C14" s="12"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C15" s="12"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
+      <c r="C14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="91.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="12"/>
-      <c r="D16" s="14"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="14"/>
       <c r="F16" s="15"/>
     </row>
-    <row r="17" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C17" s="12"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D17" s="14"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="12"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C19" s="12"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="12"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="12"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C22" s="12"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C23" s="12"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+    </row>
+    <row r="24" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C24" s="12"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+    </row>
+    <row r="25" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C25" s="12"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C26" s="12"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="7"/>
@@ -924,42 +968,42 @@
       <c r="E46" s="6"/>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="7"/>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="7"/>
@@ -5693,6 +5737,46 @@
       <c r="D1000" s="6"/>
       <c r="E1000" s="6"/>
       <c r="F1000" s="7"/>
+    </row>
+    <row r="1001" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1001" s="6"/>
+      <c r="E1001" s="6"/>
+      <c r="F1001" s="7"/>
+    </row>
+    <row r="1002" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1002" s="6"/>
+      <c r="E1002" s="6"/>
+      <c r="F1002" s="7"/>
+    </row>
+    <row r="1003" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1003" s="6"/>
+      <c r="E1003" s="6"/>
+      <c r="F1003" s="7"/>
+    </row>
+    <row r="1004" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1004" s="6"/>
+      <c r="E1004" s="6"/>
+      <c r="F1004" s="7"/>
+    </row>
+    <row r="1005" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1005" s="6"/>
+      <c r="E1005" s="6"/>
+      <c r="F1005" s="7"/>
+    </row>
+    <row r="1006" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1006" s="6"/>
+      <c r="E1006" s="6"/>
+      <c r="F1006" s="7"/>
+    </row>
+    <row r="1007" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1007" s="6"/>
+      <c r="E1007" s="6"/>
+      <c r="F1007" s="7"/>
+    </row>
+    <row r="1008" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1008" s="6"/>
+      <c r="E1008" s="6"/>
+      <c r="F1008" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5718,7 +5802,7 @@
       <selection pane="bottomLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.12"/>
@@ -5729,44 +5813,44 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="7"/>
@@ -5774,23 +5858,23 @@
       <c r="F2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>31</v>
+      <c r="E3" s="9" t="s">
+        <v>38</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>32</v>
+      <c r="F3" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>12</v>
@@ -5798,59 +5882,59 @@
     </row>
     <row r="4" customFormat="false" ht="37.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="B6" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F6" s="15"/>
     </row>
@@ -10840,58 +10924,58 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="92.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="50.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="36.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="19" width="50.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="36.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="6"/>
@@ -10899,13 +10983,13 @@
       <c r="F2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -10914,7 +10998,7 @@
       <c r="E3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="0" t="s">
@@ -10923,275 +11007,275 @@
     </row>
     <row r="4" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="18" t="n">
         <v>18</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="18" t="n">
         <v>19</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" customFormat="false" ht="49.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" customFormat="false" ht="49.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="18" t="n">
         <v>21</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="18" t="n">
         <v>22</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>58</v>
+      <c r="C8" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="18" t="n">
         <v>23</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>61</v>
+      <c r="C9" s="21" t="s">
+        <v>68</v>
       </c>
       <c r="D9" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="18" t="n">
+        <v>24</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="F10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="18" t="n">
         <v>25</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>67</v>
+      <c r="C11" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="77.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="18" t="n">
         <v>26</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>70</v>
+      <c r="C12" s="21" t="s">
+        <v>77</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="51.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="18" t="n">
         <v>27</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="F13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>77</v>
+      <c r="B14" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>81</v>
+      <c r="B15" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="F15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>85</v>
+      <c r="B16" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>89</v>
+      <c r="B17" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>93</v>
+      <c r="B18" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F18" s="7"/>
     </row>
@@ -16129,55 +16213,55 @@
       <selection pane="bottomLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="92.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="50.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="36.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="19" width="50.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="36.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="6"/>
@@ -16185,13 +16269,13 @@
       <c r="F2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -16200,7 +16284,7 @@
       <c r="E3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="0" t="s">
@@ -16232,31 +16316,31 @@
       <c r="F7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="16"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="13"/>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C9" s="16"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="14"/>
       <c r="E9" s="12"/>
       <c r="F9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="16"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C11" s="16"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="16"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>

</xml_diff>

<commit_message>
nettoyage des fichiers js
</commit_message>
<xml_diff>
--- a/Soutenance/Plan de tests.xlsx
+++ b/Soutenance/Plan de tests.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="142">
   <si>
     <t xml:space="preserve">Fichier JS</t>
   </si>
@@ -242,6 +242,15 @@
   </si>
   <si>
     <t xml:space="preserve">provoquer des erreurs dans les données et vérifier si le message affiché correspond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getCustomerDatas()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">récupère les datas du client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre un console.log(getCustomerDatas()) ; dans checkValidity() avec des erreurs. Cela permettra de vérifier que les données sont bonnes</t>
   </si>
   <si>
     <t xml:space="preserve">Appeler la fonction avec différentes valeurs de tests (valeurs limites, valeur vide...), et on observe la valeur retournée, avec un console.log par exemple</t>
@@ -725,10 +734,10 @@
   </sheetPr>
   <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1088,9 +1097,18 @@
       <c r="F30" s="14"/>
     </row>
     <row r="31" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C31" s="10"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
+      <c r="A31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="F31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6120,10 +6138,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>12</v>
@@ -6131,59 +6149,59 @@
     </row>
     <row r="4" customFormat="false" ht="37.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F6" s="14"/>
     </row>
@@ -11256,275 +11274,275 @@
     </row>
     <row r="4" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B4" s="19" t="n">
         <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B5" s="19" t="n">
         <v>19</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B6" s="19" t="n">
         <v>20</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="49.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B7" s="19" t="n">
         <v>21</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B8" s="19" t="n">
         <v>22</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B9" s="19" t="n">
         <v>23</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B10" s="19" t="n">
         <v>24</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B11" s="19" t="n">
         <v>25</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="77.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B12" s="19" t="n">
         <v>26</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="51.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B13" s="19" t="n">
         <v>27</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F18" s="16"/>
     </row>

</xml_diff>